<commit_message>
already parametrize with multiple vehicles
</commit_message>
<xml_diff>
--- a/Vehicles_Params_Summary.xlsx
+++ b/Vehicles_Params_Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cob_e\BEV_Modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D269114-1BB3-4750-A57C-C4EFA54FEE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C690F2-DEAD-4C84-B396-2DDE9CB5D499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1095" yWindow="1095" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery EV - Dataset" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="121">
   <si>
     <t>Parameter</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>Coulomb_Eff</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz_2</t>
   </si>
 </sst>
 </file>
@@ -530,10 +533,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -819,7 +822,7 @@
   <dimension ref="A1:AG8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +986,7 @@
       <c r="I2" t="s">
         <v>107</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="10">
         <v>3</v>
       </c>
       <c r="K2">
@@ -1367,7 +1370,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B8">
         <v>113</v>
@@ -1472,15 +1475,15 @@
       <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">

</xml_diff>